<commit_message>
Fixed IRI of annotation property prism_id
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@71247 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/prism/PRISM_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/prism/PRISM_metadata.xlsx
@@ -11072,9 +11072,6 @@
     </r>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/eupath/icemr.owl#prism_id</t>
-  </si>
-  <si>
     <t>PRISM ID</t>
   </si>
   <si>
@@ -11409,6 +11406,9 @@
   </si>
   <si>
     <t>PRISM_0000111</t>
+  </si>
+  <si>
+    <t>eupath/icemr.owl#prism_id</t>
   </si>
 </sst>
 </file>
@@ -16359,7 +16359,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -19296,7 +19296,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19333,7 +19333,7 @@
         <v>1817</v>
       </c>
       <c r="G1" s="164" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="H1" s="151" t="s">
         <v>511</v>
@@ -19355,7 +19355,7 @@
         <v>1820</v>
       </c>
       <c r="G2" s="174" t="s">
-        <v>2700</v>
+        <v>2812</v>
       </c>
       <c r="H2" s="151" t="s">
         <v>1815</v>
@@ -19381,7 +19381,7 @@
         <v>857</v>
       </c>
       <c r="G3" s="87" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="H3" s="86" t="s">
         <v>885</v>
@@ -19403,7 +19403,7 @@
       <c r="E4" s="87"/>
       <c r="F4" s="87"/>
       <c r="G4" s="87" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="H4" s="86"/>
     </row>
@@ -19423,7 +19423,7 @@
       <c r="E5" s="87"/>
       <c r="F5" s="87"/>
       <c r="G5" s="87" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="H5" s="86" t="s">
         <v>888</v>
@@ -19449,7 +19449,7 @@
         <v>673</v>
       </c>
       <c r="G6" s="87" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="H6" s="86" t="s">
         <v>744</v>
@@ -19472,7 +19472,7 @@
       <c r="E7" s="87"/>
       <c r="F7" s="87"/>
       <c r="G7" s="87" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="H7" s="86" t="s">
         <v>872</v>
@@ -19498,7 +19498,7 @@
         <v>546</v>
       </c>
       <c r="G8" s="87" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="H8" s="86" t="s">
         <v>691</v>
@@ -19521,7 +19521,7 @@
       <c r="E9" s="87"/>
       <c r="F9" s="87"/>
       <c r="G9" s="87" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="H9" s="86" t="s">
         <v>747</v>
@@ -19548,7 +19548,7 @@
         <v>858</v>
       </c>
       <c r="G10" s="87" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="H10" s="86" t="s">
         <v>887</v>
@@ -19575,7 +19575,7 @@
         <v>773</v>
       </c>
       <c r="G11" s="87" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="H11" s="86" t="s">
         <v>912</v>
@@ -19597,7 +19597,7 @@
       <c r="E12" s="87"/>
       <c r="F12" s="87"/>
       <c r="G12" s="87" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="H12" s="86" t="s">
         <v>886</v>
@@ -19624,7 +19624,7 @@
         <v>1555</v>
       </c>
       <c r="G13" s="87" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="H13" s="86" t="s">
         <v>731</v>
@@ -19651,7 +19651,7 @@
         <v>1554</v>
       </c>
       <c r="G14" s="87" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="H14" s="86" t="s">
         <v>730</v>
@@ -19674,7 +19674,7 @@
       <c r="E15" s="87"/>
       <c r="F15" s="87"/>
       <c r="G15" s="87" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="H15" s="86" t="s">
         <v>793</v>
@@ -19697,7 +19697,7 @@
       <c r="E16" s="87"/>
       <c r="F16" s="87"/>
       <c r="G16" s="87" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
       <c r="H16" s="86" t="s">
         <v>757</v>
@@ -19723,7 +19723,7 @@
         <v>1556</v>
       </c>
       <c r="G17" s="87" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
       <c r="H17" s="86" t="s">
         <v>732</v>
@@ -19750,7 +19750,7 @@
         <v>602</v>
       </c>
       <c r="G18" s="87" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="H18" s="86" t="s">
         <v>488</v>
@@ -19777,7 +19777,7 @@
         <v>868</v>
       </c>
       <c r="G19" s="87" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
       <c r="H19" s="86" t="s">
         <v>922</v>
@@ -19800,7 +19800,7 @@
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
       <c r="G20" s="87" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
       <c r="H20" s="86" t="s">
         <v>890</v>
@@ -19823,7 +19823,7 @@
       <c r="E21" s="87"/>
       <c r="F21" s="87"/>
       <c r="G21" s="87" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
       <c r="H21" s="86" t="s">
         <v>914</v>
@@ -19850,7 +19850,7 @@
         <v>774</v>
       </c>
       <c r="G22" s="87" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
       <c r="H22" s="86" t="s">
         <v>913</v>
@@ -19872,7 +19872,7 @@
       <c r="E23" s="87"/>
       <c r="F23" s="87"/>
       <c r="G23" s="87" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="H23" s="86" t="s">
         <v>889</v>
@@ -19895,7 +19895,7 @@
       <c r="E24" s="87"/>
       <c r="F24" s="87"/>
       <c r="G24" s="87" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="H24" s="86"/>
       <c r="I24" s="143"/>
@@ -19916,7 +19916,7 @@
       <c r="E25" s="87"/>
       <c r="F25" s="87"/>
       <c r="G25" s="87" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="H25" s="86"/>
       <c r="I25" s="143"/>
@@ -19941,7 +19941,7 @@
         <v>799</v>
       </c>
       <c r="G26" s="87" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="H26" s="86" t="s">
         <v>879</v>
@@ -19964,7 +19964,7 @@
       <c r="E27" s="87"/>
       <c r="F27" s="87"/>
       <c r="G27" s="87" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="H27" s="86" t="s">
         <v>892</v>
@@ -19991,7 +19991,7 @@
         <v>767</v>
       </c>
       <c r="G28" s="87" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="H28" s="86" t="s">
         <v>917</v>
@@ -20018,7 +20018,7 @@
         <v>859</v>
       </c>
       <c r="G29" s="87" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="H29" s="86" t="s">
         <v>891</v>
@@ -20045,7 +20045,7 @@
         <v>1263</v>
       </c>
       <c r="G30" s="87" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="H30" s="86" t="s">
         <v>736</v>
@@ -20072,7 +20072,7 @@
         <v>213</v>
       </c>
       <c r="G31" s="87" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="H31" s="86">
         <v>1.1000000000000001</v>
@@ -20095,7 +20095,7 @@
       <c r="E32" s="87"/>
       <c r="F32" s="87"/>
       <c r="G32" s="87" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="H32" s="86" t="s">
         <v>902</v>
@@ -20118,7 +20118,7 @@
       <c r="E33" s="87"/>
       <c r="F33" s="87"/>
       <c r="G33" s="87" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="H33" s="86" t="s">
         <v>918</v>
@@ -20144,7 +20144,7 @@
         <v>547</v>
       </c>
       <c r="G34" s="87" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="H34" s="86" t="s">
         <v>690</v>
@@ -20171,7 +20171,7 @@
         <v>669</v>
       </c>
       <c r="G35" s="87" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="H35" s="86" t="s">
         <v>739</v>
@@ -20198,7 +20198,7 @@
         <v>861</v>
       </c>
       <c r="G36" s="87" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
       <c r="H36" s="86" t="s">
         <v>897</v>
@@ -20221,7 +20221,7 @@
       <c r="E37" s="87"/>
       <c r="F37" s="87"/>
       <c r="G37" s="87" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
       <c r="H37" s="86" t="s">
         <v>896</v>
@@ -20248,7 +20248,7 @@
         <v>765</v>
       </c>
       <c r="G38" s="87" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
       <c r="H38" s="86" t="s">
         <v>884</v>
@@ -20275,7 +20275,7 @@
         <v>1798</v>
       </c>
       <c r="G39" s="87" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="H39" s="86" t="s">
         <v>726</v>
@@ -20302,7 +20302,7 @@
         <v>1794</v>
       </c>
       <c r="G40" s="87" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
       <c r="H40" s="86" t="s">
         <v>721</v>
@@ -20329,7 +20329,7 @@
         <v>1802</v>
       </c>
       <c r="G41" s="87" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="H41" s="86" t="s">
         <v>490</v>
@@ -20355,7 +20355,7 @@
         <v>856</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
       <c r="H42" s="86" t="s">
         <v>895</v>
@@ -20382,7 +20382,7 @@
         <v>553</v>
       </c>
       <c r="G43" s="87" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
       <c r="H43" s="86" t="s">
         <v>694</v>
@@ -20405,7 +20405,7 @@
       <c r="E44" s="87"/>
       <c r="F44" s="87"/>
       <c r="G44" s="87" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
       <c r="H44" s="86" t="s">
         <v>898</v>
@@ -20432,7 +20432,7 @@
         <v>554</v>
       </c>
       <c r="G45" s="87" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
       <c r="H45" s="86" t="s">
         <v>695</v>
@@ -20459,7 +20459,7 @@
         <v>1801</v>
       </c>
       <c r="G46" s="87" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
       <c r="H46" s="86" t="s">
         <v>729</v>
@@ -20486,7 +20486,7 @@
         <v>1797</v>
       </c>
       <c r="G47" s="87" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
       <c r="H47" s="86" t="s">
         <v>724</v>
@@ -20509,7 +20509,7 @@
       <c r="E48" s="87"/>
       <c r="F48" s="87"/>
       <c r="G48" s="87" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="H48" s="86" t="s">
         <v>748</v>
@@ -20532,7 +20532,7 @@
       <c r="E49" s="87"/>
       <c r="F49" s="87"/>
       <c r="G49" s="87" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
       <c r="H49" s="86" t="s">
         <v>924</v>
@@ -20555,7 +20555,7 @@
       <c r="E50" s="87"/>
       <c r="F50" s="87"/>
       <c r="G50" s="87" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="H50" s="86" t="s">
         <v>746</v>
@@ -20582,7 +20582,7 @@
         <v>1800</v>
       </c>
       <c r="G51" s="87" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="H51" s="86" t="s">
         <v>728</v>
@@ -20608,7 +20608,7 @@
         <v>1796</v>
       </c>
       <c r="G52" s="87" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
       <c r="H52" s="86" t="s">
         <v>723</v>
@@ -20630,7 +20630,7 @@
       <c r="E53" s="87"/>
       <c r="F53" s="87"/>
       <c r="G53" s="87" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="H53" s="86" t="s">
         <v>749</v>
@@ -20653,7 +20653,7 @@
       <c r="E54" s="87"/>
       <c r="F54" s="87"/>
       <c r="G54" s="87" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="H54" s="86" t="s">
         <v>900</v>
@@ -20680,7 +20680,7 @@
         <v>862</v>
       </c>
       <c r="G55" s="87" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="H55" s="86" t="s">
         <v>899</v>
@@ -20703,7 +20703,7 @@
       <c r="E56" s="87"/>
       <c r="F56" s="87"/>
       <c r="G56" s="87" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="H56" s="86" t="s">
         <v>873</v>
@@ -20729,7 +20729,7 @@
         <v>778</v>
       </c>
       <c r="G57" s="87" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="H57" s="86" t="s">
         <v>920</v>
@@ -20751,7 +20751,7 @@
       <c r="E58" s="87"/>
       <c r="F58" s="87"/>
       <c r="G58" s="87" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="H58" s="86" t="s">
         <v>741</v>
@@ -20777,7 +20777,7 @@
         <v>571</v>
       </c>
       <c r="G59" s="87" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="H59" s="86" t="s">
         <v>698</v>
@@ -20803,7 +20803,7 @@
         <v>573</v>
       </c>
       <c r="G60" s="87" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="H60" s="86" t="s">
         <v>700</v>
@@ -20829,7 +20829,7 @@
         <v>572</v>
       </c>
       <c r="G61" s="87" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="H61" s="86" t="s">
         <v>699</v>
@@ -20855,7 +20855,7 @@
         <v>541</v>
       </c>
       <c r="G62" s="87" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="H62" s="86" t="s">
         <v>687</v>
@@ -20881,7 +20881,7 @@
         <v>542</v>
       </c>
       <c r="G63" s="87" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="H63" s="86" t="s">
         <v>688</v>
@@ -20907,7 +20907,7 @@
         <v>543</v>
       </c>
       <c r="G64" s="87" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="H64" s="86" t="s">
         <v>689</v>
@@ -20933,7 +20933,7 @@
         <v>803</v>
       </c>
       <c r="G65" s="87" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="H65" s="86" t="s">
         <v>877</v>
@@ -20959,7 +20959,7 @@
         <v>860</v>
       </c>
       <c r="G66" s="87" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="H66" s="86" t="s">
         <v>893</v>
@@ -20981,7 +20981,7 @@
       <c r="E67" s="87"/>
       <c r="F67" s="87"/>
       <c r="G67" s="87" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="H67" s="86" t="s">
         <v>894</v>
@@ -21003,7 +21003,7 @@
       <c r="E68" s="87"/>
       <c r="F68" s="87"/>
       <c r="G68" s="87" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
       <c r="H68" s="86" t="s">
         <v>901</v>
@@ -21029,7 +21029,7 @@
         <v>672</v>
       </c>
       <c r="G69" s="87" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
       <c r="H69" s="86" t="s">
         <v>740</v>
@@ -21051,7 +21051,7 @@
       <c r="E70" s="87"/>
       <c r="F70" s="87"/>
       <c r="G70" s="87" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="H70" s="86" t="s">
         <v>916</v>
@@ -21077,7 +21077,7 @@
         <v>849</v>
       </c>
       <c r="G71" s="87" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
       <c r="H71" s="86" t="s">
         <v>927</v>
@@ -21099,7 +21099,7 @@
       <c r="E72" s="87"/>
       <c r="F72" s="87"/>
       <c r="G72" s="87" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
       <c r="H72" s="86" t="s">
         <v>904</v>
@@ -21125,7 +21125,7 @@
         <v>291</v>
       </c>
       <c r="G73" s="87" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="H73" s="86" t="s">
         <v>870</v>
@@ -21147,7 +21147,7 @@
       <c r="E74" s="87"/>
       <c r="F74" s="87"/>
       <c r="G74" s="87" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="H74" s="86" t="s">
         <v>903</v>
@@ -21173,7 +21173,7 @@
         <v>850</v>
       </c>
       <c r="G75" s="87" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="H75" s="86" t="s">
         <v>928</v>
@@ -21199,7 +21199,7 @@
         <v>1265</v>
       </c>
       <c r="G76" s="87" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="H76" s="86" t="s">
         <v>737</v>
@@ -21225,7 +21225,7 @@
         <v>316</v>
       </c>
       <c r="G77" s="87" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="H77" s="86" t="s">
         <v>487</v>
@@ -21251,7 +21251,7 @@
         <v>570</v>
       </c>
       <c r="G78" s="87" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="H78" s="86" t="s">
         <v>697</v>
@@ -21277,7 +21277,7 @@
         <v>1804</v>
       </c>
       <c r="G79" s="87" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="H79" s="86" t="s">
         <v>734</v>
@@ -21303,7 +21303,7 @@
         <v>1803</v>
       </c>
       <c r="G80" s="87" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="H80" s="86" t="s">
         <v>733</v>
@@ -21329,7 +21329,7 @@
         <v>537</v>
       </c>
       <c r="G81" s="87" t="s">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="H81" s="86" t="s">
         <v>686</v>
@@ -21355,7 +21355,7 @@
         <v>772</v>
       </c>
       <c r="G82" s="87" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
       <c r="H82" s="86" t="s">
         <v>923</v>
@@ -21381,7 +21381,7 @@
         <v>1264</v>
       </c>
       <c r="G83" s="87" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
       <c r="H83" s="86" t="s">
         <v>735</v>
@@ -21403,7 +21403,7 @@
       <c r="E84" s="87"/>
       <c r="F84" s="87"/>
       <c r="G84" s="87" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
       <c r="H84" s="86" t="s">
         <v>909</v>
@@ -21429,7 +21429,7 @@
         <v>549</v>
       </c>
       <c r="G85" s="87" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="H85" s="86" t="s">
         <v>692</v>
@@ -21455,7 +21455,7 @@
         <v>1903</v>
       </c>
       <c r="G86" s="87" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="H86" s="86" t="s">
         <v>925</v>
@@ -21477,7 +21477,7 @@
       <c r="E87" s="87"/>
       <c r="F87" s="87"/>
       <c r="G87" s="87" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="H87" s="86" t="s">
         <v>742</v>
@@ -21499,7 +21499,7 @@
       <c r="E88" s="87"/>
       <c r="F88" s="87"/>
       <c r="G88" s="87" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
       <c r="H88" s="86" t="s">
         <v>906</v>
@@ -21525,7 +21525,7 @@
         <v>863</v>
       </c>
       <c r="G89" s="87" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="H89" s="86" t="s">
         <v>905</v>
@@ -21551,7 +21551,7 @@
         <v>559</v>
       </c>
       <c r="G90" s="87" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="H90" s="86" t="s">
         <v>696</v>
@@ -21573,7 +21573,7 @@
       <c r="E91" s="87"/>
       <c r="F91" s="87"/>
       <c r="G91" s="87" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="H91" s="86" t="s">
         <v>915</v>
@@ -21599,7 +21599,7 @@
         <v>558</v>
       </c>
       <c r="G92" s="87" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="H92" s="86" t="s">
         <v>482</v>
@@ -21625,7 +21625,7 @@
         <v>867</v>
       </c>
       <c r="G93" s="87" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="H93" s="86" t="s">
         <v>919</v>
@@ -21651,7 +21651,7 @@
         <v>565</v>
       </c>
       <c r="G94" s="87" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="H94" s="86" t="s">
         <v>499</v>
@@ -21677,7 +21677,7 @@
         <v>561</v>
       </c>
       <c r="G95" s="87" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="H95" s="86" t="s">
         <v>491</v>
@@ -21704,7 +21704,7 @@
         <v>676</v>
       </c>
       <c r="G96" s="87" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="H96" s="86" t="s">
         <v>738</v>
@@ -21727,7 +21727,7 @@
       <c r="E97" s="87"/>
       <c r="F97" s="87"/>
       <c r="G97" s="87" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="H97" s="86" t="s">
         <v>753</v>
@@ -21749,7 +21749,7 @@
       <c r="E98" s="87"/>
       <c r="F98" s="87"/>
       <c r="G98" s="87" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="H98" s="86" t="s">
         <v>758</v>
@@ -21772,7 +21772,7 @@
       <c r="E99" s="87"/>
       <c r="F99" s="87"/>
       <c r="G99" s="87" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="H99" s="86" t="s">
         <v>755</v>
@@ -21799,7 +21799,7 @@
         <v>1559</v>
       </c>
       <c r="G100" s="87" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="H100" s="86" t="s">
         <v>489</v>
@@ -21826,7 +21826,7 @@
         <v>1557</v>
       </c>
       <c r="G101" s="87" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="H101" s="86" t="s">
         <v>725</v>
@@ -21853,7 +21853,7 @@
         <v>1558</v>
       </c>
       <c r="G102" s="87" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="H102" s="86" t="s">
         <v>720</v>
@@ -21880,7 +21880,7 @@
         <v>1799</v>
       </c>
       <c r="G103" s="87" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="H103" s="86" t="s">
         <v>727</v>
@@ -21907,7 +21907,7 @@
         <v>1795</v>
       </c>
       <c r="G104" s="87" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="H104" s="86" t="s">
         <v>722</v>
@@ -21930,7 +21930,7 @@
       <c r="E105" s="87"/>
       <c r="F105" s="87"/>
       <c r="G105" s="87" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="H105" s="86" t="s">
         <v>908</v>
@@ -21953,7 +21953,7 @@
       <c r="E106" s="87"/>
       <c r="F106" s="87"/>
       <c r="G106" s="87" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="H106" s="86" t="s">
         <v>754</v>
@@ -21975,7 +21975,7 @@
       <c r="E107" s="87"/>
       <c r="F107" s="87"/>
       <c r="G107" s="87" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="H107" s="86" t="s">
         <v>792</v>
@@ -21997,7 +21997,7 @@
       <c r="E108" s="87"/>
       <c r="F108" s="87"/>
       <c r="G108" s="87" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="H108" s="86" t="s">
         <v>756</v>
@@ -22023,7 +22023,7 @@
         <v>864</v>
       </c>
       <c r="G109" s="87" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="H109" s="86" t="s">
         <v>907</v>
@@ -22050,7 +22050,7 @@
         <v>550</v>
       </c>
       <c r="G110" s="87" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="H110" s="86" t="s">
         <v>693</v>
@@ -22077,7 +22077,7 @@
         <v>564</v>
       </c>
       <c r="G111" s="87" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="H111" s="86" t="s">
         <v>498</v>
@@ -22100,7 +22100,7 @@
       <c r="E112" s="87"/>
       <c r="F112" s="87"/>
       <c r="G112" s="87" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="H112" s="86" t="s">
         <v>874</v>
@@ -22122,7 +22122,7 @@
       <c r="E113" s="87"/>
       <c r="F113" s="87"/>
       <c r="G113" s="87" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="H113" s="86" t="s">
         <v>743</v>
@@ -23011,7 +23011,7 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="A144" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2" location="prism_id"/>
+    <hyperlink ref="G2" r:id="rId2" location="prism_id" display="http://purl.obolibrary.org/obo/eupath/icemr.owl#prism_id"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>